<commit_message>
favorised tp1 with tp2 than tp1 with td2(and the opposite)
</commit_message>
<xml_diff>
--- a/modele/Tous_les_Emplois_du_Temps.xlsx
+++ b/modele/Tous_les_Emplois_du_Temps.xlsx
@@ -572,11 +572,25 @@
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="5" t="inlineStr"/>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -612,14 +626,7 @@
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
       <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -650,14 +657,7 @@
           <t>17:00-18:30</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
@@ -758,14 +758,7 @@
       </c>
       <c r="B3" s="5" t="inlineStr"/>
       <c r="C3" s="5" t="inlineStr"/>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
       <c r="G3" s="5" t="inlineStr"/>
@@ -800,7 +793,14 @@
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
       <c r="F5" s="5" t="inlineStr"/>
@@ -820,7 +820,14 @@
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="F6" s="5" t="inlineStr"/>
       <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
@@ -837,14 +844,7 @@
       </c>
       <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
       <c r="G7" s="5" t="inlineStr"/>
@@ -946,14 +946,7 @@
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1021,7 +1014,8 @@
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr"/>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1029,9 +1023,15 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
@@ -1155,7 +1155,23 @@
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="6" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1163,22 +1179,6 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
       <c r="F5" s="5" t="inlineStr"/>
       <c r="G5" s="5" t="inlineStr"/>
@@ -1656,49 +1656,48 @@
       <c r="B3" s="7" t="inlineStr">
         <is>
           <t>[RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV310] POO JAVA
-(CM)
-Prof: Esseyssah
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>[DAS310] Maching Learning
-(CM)
-Prof: Louly
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
 (TD) - TD1
 Prof: Aloun
+Salle: 101 /// [DAS311] RO
+(TD) - TD2
+Prof: abderrahmane
+Salle: 102</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>[PAV311] SD &amp; Comp.Algo
+(CM)
+Prof: Meyara
 Salle: 101</t>
         </is>
       </c>
-      <c r="F3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 201</t>
+      <c r="E3" s="5" t="inlineStr"/>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>[RSS311] Administration reseaux
+(TP) - TD1
+Prof: Aloun
+Salle: 102 /// [DAS311] RO
+(TP) - TD2
+Prof: abderrahmane
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 102</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
@@ -1713,19 +1712,19 @@
           <t>09:45-11:15</t>
         </is>
       </c>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TP) - TD2
-Prof: abderrahmane
-Salle: 102</t>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>[DPR310] Communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
         </is>
       </c>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>[RSS310] Reseaux Mobile
-(CM)
-Prof: Aloun
+          <t>[PAV310] POO JAVA
+(CM)
+Prof: Esseyssah
 Salle: 101</t>
         </is>
       </c>
@@ -1734,26 +1733,22 @@
           <t>[DAS311] RO
 (TP) - TD1
 Prof: abderrahmane
-Salle: 102</t>
+Salle: 102 /// [RSS311] Administration reseaux
+(TP) - TD2
+Prof: Aloun
+Salle: 103</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr"/>
       <c r="F4" s="6" t="inlineStr">
         <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="G4" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
+          <t>[DAS311] RO
+(CM)
+Prof: Cheikh
 Salle: 101</t>
         </is>
       </c>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1769,18 +1764,21 @@
       <c r="B5" s="5" t="inlineStr"/>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>[RSS311] Administration reseaux
-(CM)
+          <t>[DPR313] Gestion d'enterprise
+(CM)
+Prof: El Bennany
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 102 /// [RSS310] Reseaux Mobile
+(TD) - TD2
 Prof: Aloun
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D5" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 101</t>
+Salle: 103</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
@@ -1794,10 +1792,10 @@
       <c r="F5" s="5" t="inlineStr"/>
       <c r="G5" s="6" t="inlineStr">
         <is>
-          <t>[PAV311] SD &amp; Comp.Algo
-(CM)
-Prof: Meyara
-Salle: 201</t>
+          <t>[DPR310] Communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
@@ -1826,37 +1824,34 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>[DAS311] RO
-(CM)
-Prof: Cheikh
+          <t>[RSS321] BD &amp; CSI
+(CM)
+Prof: Med Lemine
 Salle: 101</t>
         </is>
       </c>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
+          <t>[DAS310] Maching Learning
+(CM)
+Prof: Louly
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>[DPR311] Anglais
+(CM)
+Prof: Blake
 Salle: 101</t>
         </is>
       </c>
-      <c r="F6" s="8" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 101 /// [RSS311] Administration reseaux
-(TP) - TD2
-Prof: Aloun
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
-        <is>
-          <t>[RSS311] Administration reseaux
-(TP) - TD1
-Prof: Aloun
-Salle: 102</t>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 101</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr">
@@ -1873,10 +1868,10 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>[DPR313] Gestion d'enterprise
-(CM)
-Prof: El Bennany
-Salle: 201</t>
+          <t>[RSS311] Administration reseaux
+(CM)
+Prof: Aloun
+Salle: 101</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
@@ -1884,44 +1879,37 @@
           <t>[RSS310] Reseaux Mobile
 (TD) - TD1
 Prof: Aloun
-Salle: 102 /// [DAS311] RO
+Salle: 101 /// [DAS311] RO
 (TD) - TD2
 Prof: abderrahmane
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="D7" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
 Salle: 102</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>[RSS321] BD &amp; CSI
+(CM)
+Prof: Med Lemine
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR311] Anglais
+(CM)
+Prof: Blake
 Salle: 101</t>
         </is>
       </c>
       <c r="F7" s="6" t="inlineStr">
         <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+          <t>[RSS310] Reseaux Mobile
+(CM)
+Prof: Aloun
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>

<commit_message>
generated a test timetable
</commit_message>
<xml_diff>
--- a/modele/Tous_les_Emplois_du_Temps.xlsx
+++ b/modele/Tous_les_Emplois_du_Temps.xlsx
@@ -572,7 +572,87 @@
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="6" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr"/>
+      <c r="D3" s="5" t="inlineStr"/>
+      <c r="E3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="80" customHeight="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>09:45-11:15</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr"/>
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr"/>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr"/>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -580,10 +660,29 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr"/>
-      <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="6" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>17:00-18:30</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -591,78 +690,19 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="80" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>09:45-11:15</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr"/>
-      <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="5" t="inlineStr"/>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr"/>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr"/>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="80" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>17:00-18:30</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -760,8 +800,16 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -776,24 +824,7 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="5" t="inlineStr"/>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -801,26 +832,32 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr"/>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr"/>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -828,8 +865,43 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr"/>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -846,8 +918,16 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -942,11 +1022,26 @@
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="5" t="inlineStr"/>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -959,12 +1054,27 @@
           <t>09:45-11:15</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -981,8 +1091,16 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -999,8 +1117,16 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1015,24 +1141,18 @@
       </c>
       <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1130,8 +1250,16 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1146,7 +1274,32 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="5" t="inlineStr"/>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1154,24 +1307,58 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="6" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr"/>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>17:00-18:30</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr"/>
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1179,45 +1366,18 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr"/>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="80" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>17:00-18:30</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr"/>
-      <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1315,8 +1475,16 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1333,8 +1501,16 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1351,8 +1527,16 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1369,8 +1553,16 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1387,8 +1579,16 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1486,8 +1686,16 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1504,8 +1712,16 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1522,8 +1738,16 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1540,8 +1764,16 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1558,8 +1790,16 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1655,33 +1895,16 @@
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>[RSS310] Reseaux Mobile
+          <t>[DAS311] RO
 (TD) - TD1
+Prof: abderrahmane
+Salle: 101 /// [RSS310] Reseaux Mobile
+(TD) - TD2
 Prof: Aloun
-Salle: 101 /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
 Salle: 102</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV311] SD &amp; Comp.Algo
-(CM)
-Prof: Meyara
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="8" t="inlineStr">
+      <c r="C3" s="8" t="inlineStr">
         <is>
           <t>[RSS311] Administration reseaux
 (TP) - TD1
@@ -1692,43 +1915,148 @@
 Salle: 103</t>
         </is>
       </c>
-      <c r="G3" s="7" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>[RSS310] Reseaux Mobile
+(CM)
+Prof: Aloun
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="80" customHeight="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>09:45-11:15</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>[RSS321] BD &amp; CSI
+(CM)
+Prof: Med Lemine
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>[RSS310] Reseaux Mobile
+(TD) - TD1
+Prof: Aloun
+Salle: 102 /// [DAS311] RO
+(TD) - TD2
+Prof: abderrahmane
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>[PAV311] SD &amp; Comp.Algo
+(CM)
+Prof: Meyara
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>[RSS310] Reseaux Mobile
+(TD) - TD1
+Prof: Aloun
+Salle: 102 /// [DAS311] RO
+(TD) - TD2
+Prof: abderrahmane
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
         <is>
           <t>[DAS311] RO
 (TD) - TD1
 Prof: abderrahmane
+Salle: 101 /// [RSS310] Reseaux Mobile
+(TD) - TD2
+Prof: Aloun
 Salle: 102</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="80" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>09:45-11:15</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>[PAV310] POO JAVA
-(CM)
-Prof: Esseyssah
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D4" s="8" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>[DAS311] RO
 (TP) - TD1
@@ -1739,8 +2067,15 @@
 Salle: 103</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="6" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>[PAV310] POO JAVA
+(CM)
+Prof: Esseyssah
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>[DAS311] RO
 (CM)
@@ -1748,49 +2083,53 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>[DPR313] Gestion d'enterprise
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>[DPR311] Anglais
 (CM)
-Prof: El Bennany
+Prof: Blake
 Salle: 201</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>17:00-18:30</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>[DAS310] Maching Learning
+(CM)
+Prof: Louly
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>[DAS311] RO
 (TD) - TD2
 Prof: abderrahmane
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="6" t="inlineStr">
+Salle: 102</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>[DPR310] Communication
 (CM)
@@ -1798,31 +2137,7 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 101 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="6" t="inlineStr">
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>[RSS321] BD &amp; CSI
 (CM)
@@ -1830,86 +2145,16 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>[DAS310] Maching Learning
-(CM)
-Prof: Louly
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="80" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>17:00-18:30</t>
-        </is>
-      </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[RSS311] Administration reseaux
-(CM)
-Prof: Aloun
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
-(TD) - TD1
-Prof: Aloun
-Salle: 101 /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="D7" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="E7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
-(CM)
-Prof: Aloun
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2007,8 +2252,16 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2025,8 +2278,16 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr"/>
-      <c r="G4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2043,8 +2304,16 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2061,8 +2330,16 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2079,8 +2356,16 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>

<commit_message>
created the stats graphs and made a real dashboard
</commit_message>
<xml_diff>
--- a/modele/Tous_les_Emplois_du_Temps.xlsx
+++ b/modele/Tous_les_Emplois_du_Temps.xlsx
@@ -572,17 +572,23 @@
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="5" t="inlineStr"/>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
@@ -601,16 +607,8 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -627,16 +625,8 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -652,24 +642,9 @@
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -682,27 +657,12 @@
           <t>17:00-18:30</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -800,16 +760,8 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -824,7 +776,24 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="5" t="inlineStr"/>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -832,50 +801,10 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -891,17 +820,16 @@
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -918,16 +846,8 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1022,26 +942,11 @@
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1054,27 +959,12 @@
           <t>09:45-11:15</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1091,16 +981,8 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1117,16 +999,8 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1141,18 +1015,24 @@
       </c>
       <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="5" t="inlineStr"/>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1250,16 +1130,8 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1274,18 +1146,17 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="5" t="inlineStr"/>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1299,7 +1170,8 @@
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1307,18 +1179,9 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1335,16 +1198,8 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1358,26 +1213,11 @@
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr"/>
-      <c r="C7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1475,16 +1315,8 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1501,16 +1333,8 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1527,16 +1351,8 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1553,16 +1369,8 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1579,16 +1387,8 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1686,16 +1486,8 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1712,16 +1504,8 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1738,16 +1522,8 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1764,16 +1540,8 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1790,16 +1558,8 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1895,6 +1655,163 @@
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
+          <t>[RSS310] Reseaux Mobile
+(TD) - TD1
+Prof: Aloun
+Salle: 101 /// [DAS311] RO
+(TD) - TD2
+Prof: abderrahmane
+Salle: 102</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>[PAV311] SD &amp; Comp.Algo
+(CM)
+Prof: Meyara
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr"/>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>[RSS311] Administration reseaux
+(TP) - TD1
+Prof: Aloun
+Salle: 102 /// [DAS311] RO
+(TP) - TD2
+Prof: abderrahmane
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 102</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="80" customHeight="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>09:45-11:15</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>[DPR310] Communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>[PAV310] POO JAVA
+(CM)
+Prof: Esseyssah
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TP) - TD1
+Prof: abderrahmane
+Salle: 102 /// [RSS311] Administration reseaux
+(TP) - TD2
+Prof: Aloun
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(CM)
+Prof: Cheikh
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr"/>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>[DPR313] Gestion d'enterprise
+(CM)
+Prof: El Bennany
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 102 /// [RSS310] Reseaux Mobile
+(TD) - TD2
+Prof: Aloun
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD2
+Prof: abderrahmane
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>[DPR310] Communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
           <t>[DAS311] RO
 (TD) - TD1
 Prof: abderrahmane
@@ -1904,226 +1821,65 @@
 Salle: 102</t>
         </is>
       </c>
-      <c r="C3" s="8" t="inlineStr">
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>[RSS321] BD &amp; CSI
+(CM)
+Prof: Med Lemine
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>[DAS310] Maching Learning
+(CM)
+Prof: Louly
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>[DPR311] Anglais
+(CM)
+Prof: Blake
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>17:00-18:30</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>[RSS311] Administration reseaux
-(TP) - TD1
-Prof: Aloun
-Salle: 102 /// [DAS311] RO
-(TP) - TD2
-Prof: abderrahmane
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
 (CM)
 Prof: Aloun
 Salle: 101</t>
         </is>
       </c>
-      <c r="E3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="80" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>09:45-11:15</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>[RSS310] Reseaux Mobile
 (TD) - TD1
 Prof: Aloun
-Salle: 102 /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>[PAV311] SD &amp; Comp.Algo
-(CM)
-Prof: Meyara
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
-(TD) - TD1
-Prof: Aloun
-Salle: 102 /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 101 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="8" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TP) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS311] Administration reseaux
-(TP) - TD2
-Prof: Aloun
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>[PAV310] POO JAVA
-(CM)
-Prof: Esseyssah
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(CM)
-Prof: Cheikh
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="80" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>17:00-18:30</t>
-        </is>
-      </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[DAS310] Maching Learning
-(CM)
-Prof: Louly
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
+Salle: 101 /// [DAS311] RO
 (TD) - TD2
 Prof: abderrahmane
 Salle: 102</t>
@@ -2131,30 +1887,29 @@
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
+          <t>[RSS321] BD &amp; CSI
+(CM)
+Prof: Med Lemine
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR311] Anglais
+(CM)
+Prof: Blake
 Salle: 101</t>
         </is>
       </c>
-      <c r="E7" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>[RSS310] Reseaux Mobile
+(CM)
+Prof: Aloun
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2252,16 +2007,8 @@
       <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2278,16 +2025,8 @@
       <c r="C4" s="5" t="inlineStr"/>
       <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2304,16 +2043,8 @@
       <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2330,16 +2061,8 @@
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
       <c r="E6" s="5" t="inlineStr"/>
-      <c r="F6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -2356,16 +2079,8 @@
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>

<commit_message>
Version te3btni, 2lmouhim: i've succefully implimented an online class through the specification button on the weekly workload, the only thing changed on the optimization file is simply adding the online classes variables nothing else no logic no mathamathical equation changed, and just a simple dropdown to filter the semesters and finally added a clean version of sql that will not show any error. 7tte description commit te3btni
</commit_message>
<xml_diff>
--- a/modele/Tous_les_Emplois_du_Temps.xlsx
+++ b/modele/Tous_les_Emplois_du_Temps.xlsx
@@ -572,25 +572,11 @@
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr"/>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="C3" s="5" t="inlineStr"/>
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -626,7 +612,14 @@
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
       <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -662,7 +655,14 @@
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
+      <c r="G7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -793,14 +793,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="C5" s="5" t="inlineStr"/>
       <c r="D5" s="5" t="inlineStr"/>
       <c r="E5" s="5" t="inlineStr"/>
       <c r="F5" s="5" t="inlineStr"/>
@@ -820,7 +813,22 @@
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>17:00-18:30</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -828,23 +836,15 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr"/>
-      <c r="G6" s="5" t="inlineStr"/>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="80" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>17:00-18:30</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="5" t="inlineStr"/>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
       <c r="G7" s="5" t="inlineStr"/>
@@ -946,7 +946,14 @@
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr"/>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1014,8 +1021,7 @@
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr"/>
-      <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="6" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1023,15 +1029,9 @@
 Salle: 101</t>
         </is>
       </c>
+      <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="F7" s="5" t="inlineStr"/>
       <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
@@ -1171,7 +1171,26 @@
       </c>
       <c r="B5" s="5" t="inlineStr"/>
       <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="6" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr"/>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1179,25 +1198,6 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr"/>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr"/>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="5" t="inlineStr"/>
       <c r="F6" s="5" t="inlineStr"/>
       <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
@@ -1653,7 +1653,138 @@
           <t>08:00-09:30</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>[RSS310] Reseaux Mobile
+(CM)
+Prof: Aloun
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 101 /// [RSS310] Reseaux Mobile
+(TD) - TD2
+Prof: Aloun
+Salle: 102</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>[DPR310] Communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>[RSS320] Introduction a la securite
+(TP) - TD1
+Prof: Tourad
+Salle: 102 /// [DAS311] RO
+(TP) - TD2
+Prof: abderrahmane
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 102 /// [RSS320] Introduction a la securite
+(TD) - TD2
+Prof: Tourad
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="80" customHeight="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>09:45-11:15</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>[DPR310] Communication
+(CM Online)
+Prof: Dieynaba
+Salle: En ligne</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>[RSS311] Administration reseaux
+(CM)
+Prof: Aloun
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>[PAV311] SD &amp; Comp.Algo
+(CM)
+Prof: Meyara
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr"/>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>[RSS321] BD &amp; CSI
+(CM)
+Prof: Med Lemine
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
+        <is>
+          <t>[PAV312] Projet Integrateur
+(CM)
+Prof: Encadreur
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="80" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>11:30-13:00</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>[DAS310] Maching Learning
+(CM Online)
+Prof: Louly
+Salle: En ligne</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
         <is>
           <t>[RSS310] Reseaux Mobile
 (TD) - TD1
@@ -1664,217 +1795,7 @@
 Salle: 102</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV311] SD &amp; Comp.Algo
-(CM)
-Prof: Meyara
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="E3" s="5" t="inlineStr"/>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>[RSS311] Administration reseaux
-(TP) - TD1
-Prof: Aloun
-Salle: 102 /// [DAS311] RO
-(TP) - TD2
-Prof: abderrahmane
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="G3" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="H3" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="80" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>09:45-11:15</t>
-        </is>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>[PAV310] POO JAVA
-(CM)
-Prof: Esseyssah
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D4" s="8" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TP) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS311] Administration reseaux
-(TP) - TD2
-Prof: Aloun
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="6" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(CM)
-Prof: Cheikh
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr"/>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="80" customHeight="1">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>11:30-13:00</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>[DPR313] Gestion d'enterprise
-(CM)
-Prof: El Bennany
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 103</t>
-        </is>
-      </c>
       <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="6" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="H5" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="80" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>15:00-16:30</t>
-        </is>
-      </c>
-      <c r="B6" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 101 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="inlineStr"/>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>[DAS310] Maching Learning
-(CM)
-Prof: Louly
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="H6" s="5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="80" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>17:00-18:30</t>
-        </is>
-      </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[RSS311] Administration reseaux
-(CM)
-Prof: Aloun
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>[RSS310] Reseaux Mobile
 (TD) - TD1
@@ -1885,7 +1806,61 @@
 Salle: 102</t>
         </is>
       </c>
-      <c r="D7" s="6" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr"/>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t>[RSS311] Administration reseaux
+(TP) - TD1
+Prof: Aloun
+Salle: 102 /// [RSS320] Introduction a la securite
+(TP) - TD2
+Prof: Tourad
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="80" customHeight="1">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>15:00-16:30</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>[RSS321] BD &amp; CSI
+(TD Online) - TD1
+Prof: Med Lemine
+Salle: En ligne /// [DAS311] RO
+(TD) - TD2
+Prof: abderrahmane
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>[RSS320] Introduction a la securite
+(TD) - TD1
+Prof: Tourad
+Salle: 101 /// [RSS310] Reseaux Mobile
+(TD) - TD2
+Prof: Aloun
+Salle: 102</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(CM)
+Prof: Cheikh
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>[RSS321] BD &amp; CSI
 (CM)
@@ -1893,7 +1868,7 @@
 Salle: 201</t>
         </is>
       </c>
-      <c r="E7" s="6" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>[DPR311] Anglais
 (CM)
@@ -1901,15 +1876,83 @@
 Salle: 101</t>
         </is>
       </c>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>[PAV310] POO JAVA
+(CM)
+Prof: Esseyssah
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="80" customHeight="1">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>17:00-18:30</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR313] Gestion d'enterprise
+(CM)
+Prof: El Bennany
+Salle: 201</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>[RSS320] Introduction a la securite
+(TP) - TD1
+Prof: Tourad
+Salle: 102 /// [RSS311] Administration reseaux
+(TP) - TD2
+Prof: Aloun
+Salle: 103</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TD) - TD1
+Prof: abderrahmane
+Salle: 102 /// [RSS321] BD &amp; CSI
+(TD Online) - TD2
+Prof: Med Lemine
+Salle: En ligne</t>
+        </is>
+      </c>
+      <c r="E7" s="8" t="inlineStr">
+        <is>
+          <t>[DAS311] RO
+(TP) - TD1
+Prof: abderrahmane
+Salle: 102 /// [RSS320] Introduction a la securite
+(TP) - TD2
+Prof: Tourad
+Salle: 103</t>
+        </is>
+      </c>
       <c r="F7" s="6" t="inlineStr">
         <is>
-          <t>[RSS310] Reseaux Mobile
+          <t>[DPR310] Communication
 (CM)
-Prof: Aloun
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="inlineStr">
+        <is>
+          <t>[DAS310] Maching Learning
+(CM)
+Prof: Louly
 Salle: 201</t>
         </is>
       </c>
-      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>

<commit_message>
fix the online course logic
</commit_message>
<xml_diff>
--- a/modele/Tous_les_Emplois_du_Temps.xlsx
+++ b/modele/Tous_les_Emplois_du_Temps.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="G1-L1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="G2-L1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="G3-L1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="G4-L1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="DSI1-L2" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="DSI2-L2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="RSS-L2" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="DWM-L2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G1-L1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G2-L1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G3-L1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G4-L1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DSI1-L2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DSI2-L2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RSS-L2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DWM-L2" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -45,7 +45,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -72,20 +72,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFE699"/>
-        <bgColor rgb="00FFE699"/>
+        <fgColor rgb="00D6EAF8"/>
+        <bgColor rgb="00D6EAF8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00B4C7E7"/>
-        <bgColor rgb="00B4C7E7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C6E0B4"/>
-        <bgColor rgb="00C6E0B4"/>
+        <fgColor rgb="00FFE699"/>
+        <bgColor rgb="00FFE699"/>
       </patternFill>
     </fill>
   </fills>
@@ -107,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -128,9 +122,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,9 +606,9 @@
       <c r="G5" s="6" t="inlineStr">
         <is>
           <t>[DPR110] communication
-(CM)
+(CM Online)
 Prof: Dieynaba
-Salle: 101</t>
+Salle: En ligne</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
@@ -650,19 +641,19 @@
           <t>17:00-18:30</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr"/>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM Online)
+Prof: Dieynaba
+Salle: En ligne</t>
+        </is>
+      </c>
       <c r="C7" s="5" t="inlineStr"/>
       <c r="D7" s="5" t="inlineStr"/>
       <c r="E7" s="5" t="inlineStr"/>
       <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -758,7 +749,14 @@
       </c>
       <c r="B3" s="5" t="inlineStr"/>
       <c r="C3" s="5" t="inlineStr"/>
-      <c r="D3" s="5" t="inlineStr"/>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>[DPR110] communication
+(CM)
+Prof: Dieynaba
+Salle: 101</t>
+        </is>
+      </c>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
       <c r="G3" s="5" t="inlineStr"/>
@@ -828,16 +826,9 @@
           <t>17:00-18:30</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR110] communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="B7" s="5" t="inlineStr"/>
       <c r="C7" s="5" t="inlineStr"/>
-      <c r="D7" s="6" t="inlineStr">
+      <c r="D7" s="7" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -946,7 +937,7 @@
       <c r="D3" s="5" t="inlineStr"/>
       <c r="E3" s="5" t="inlineStr"/>
       <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="6" t="inlineStr">
+      <c r="G3" s="7" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1021,7 +1012,11 @@
         </is>
       </c>
       <c r="B7" s="5" t="inlineStr"/>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="5" t="inlineStr"/>
+      <c r="E7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="7" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1029,10 +1024,6 @@
 Salle: 101</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr"/>
-      <c r="E7" s="5" t="inlineStr"/>
-      <c r="F7" s="5" t="inlineStr"/>
-      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1146,7 +1137,7 @@
       </c>
       <c r="B4" s="5" t="inlineStr"/>
       <c r="C4" s="5" t="inlineStr"/>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1190,7 +1181,7 @@
       <c r="B6" s="5" t="inlineStr"/>
       <c r="C6" s="5" t="inlineStr"/>
       <c r="D6" s="5" t="inlineStr"/>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="E6" s="7" t="inlineStr">
         <is>
           <t>[DPR110] communication
 (CM)
@@ -1653,63 +1644,12 @@
           <t>08:00-09:30</t>
         </is>
       </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
-(CM)
-Prof: Aloun
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 101 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="E3" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>[RSS320] Introduction a la securite
-(TP) - TD1
-Prof: Tourad
-Salle: 102 /// [DAS311] RO
-(TP) - TD2
-Prof: abderrahmane
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="G3" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS320] Introduction a la securite
-(TD) - TD2
-Prof: Tourad
-Salle: 103</t>
-        </is>
-      </c>
+      <c r="B3" s="5" t="inlineStr"/>
+      <c r="C3" s="5" t="inlineStr"/>
+      <c r="D3" s="5" t="inlineStr"/>
+      <c r="E3" s="5" t="inlineStr"/>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1722,47 +1662,12 @@
           <t>09:45-11:15</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM Online)
-Prof: Dieynaba
-Salle: En ligne</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>[RSS311] Administration reseaux
-(CM)
-Prof: Aloun
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>[PAV311] SD &amp; Comp.Algo
-(CM)
-Prof: Meyara
-Salle: 201</t>
-        </is>
-      </c>
+      <c r="B4" s="5" t="inlineStr"/>
+      <c r="C4" s="5" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr"/>
       <c r="E4" s="5" t="inlineStr"/>
-      <c r="F4" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G4" s="6" t="inlineStr">
-        <is>
-          <t>[PAV312] Projet Integrateur
-(CM)
-Prof: Encadreur
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="F4" s="5" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1776,48 +1681,11 @@
         </is>
       </c>
       <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>[DAS310] Maching Learning
-(CM Online)
-Prof: Louly
-Salle: En ligne</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
-(TD) - TD1
-Prof: Aloun
-Salle: 101 /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>[RSS310] Reseaux Mobile
-(TD) - TD1
-Prof: Aloun
-Salle: 101 /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 102</t>
-        </is>
-      </c>
+      <c r="C5" s="5" t="inlineStr"/>
+      <c r="D5" s="5" t="inlineStr"/>
+      <c r="E5" s="5" t="inlineStr"/>
       <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="8" t="inlineStr">
-        <is>
-          <t>[RSS311] Administration reseaux
-(TP) - TD1
-Prof: Aloun
-Salle: 102 /// [RSS320] Introduction a la securite
-(TP) - TD2
-Prof: Tourad
-Salle: 103</t>
-        </is>
-      </c>
+      <c r="G5" s="5" t="inlineStr"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1830,60 +1698,12 @@
           <t>15:00-16:30</t>
         </is>
       </c>
-      <c r="B6" s="7" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(TD Online) - TD1
-Prof: Med Lemine
-Salle: En ligne /// [DAS311] RO
-(TD) - TD2
-Prof: abderrahmane
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="C6" s="7" t="inlineStr">
-        <is>
-          <t>[RSS320] Introduction a la securite
-(TD) - TD1
-Prof: Tourad
-Salle: 101 /// [RSS310] Reseaux Mobile
-(TD) - TD2
-Prof: Aloun
-Salle: 102</t>
-        </is>
-      </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(CM)
-Prof: Cheikh
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>[RSS321] BD &amp; CSI
-(CM)
-Prof: Med Lemine
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="F6" s="6" t="inlineStr">
-        <is>
-          <t>[DPR311] Anglais
-(CM)
-Prof: Blake
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G6" s="6" t="inlineStr">
-        <is>
-          <t>[PAV310] POO JAVA
-(CM)
-Prof: Esseyssah
-Salle: 101</t>
-        </is>
-      </c>
+      <c r="B6" s="5" t="inlineStr"/>
+      <c r="C6" s="5" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr"/>
+      <c r="E6" s="5" t="inlineStr"/>
+      <c r="F6" s="5" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
           <t>x</t>
@@ -1896,63 +1716,12 @@
           <t>17:00-18:30</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR313] Gestion d'enterprise
-(CM)
-Prof: El Bennany
-Salle: 201</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="inlineStr">
-        <is>
-          <t>[RSS320] Introduction a la securite
-(TP) - TD1
-Prof: Tourad
-Salle: 102 /// [RSS311] Administration reseaux
-(TP) - TD2
-Prof: Aloun
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="D7" s="7" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TD) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS321] BD &amp; CSI
-(TD Online) - TD2
-Prof: Med Lemine
-Salle: En ligne</t>
-        </is>
-      </c>
-      <c r="E7" s="8" t="inlineStr">
-        <is>
-          <t>[DAS311] RO
-(TP) - TD1
-Prof: abderrahmane
-Salle: 102 /// [RSS320] Introduction a la securite
-(TP) - TD2
-Prof: Tourad
-Salle: 103</t>
-        </is>
-      </c>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>[DPR310] Communication
-(CM)
-Prof: Dieynaba
-Salle: 101</t>
-        </is>
-      </c>
-      <c r="G7" s="6" t="inlineStr">
-        <is>
-          <t>[DAS310] Maching Learning
-(CM)
-Prof: Louly
-Salle: 201</t>
-        </is>
-      </c>
+      <c r="B7" s="5" t="inlineStr"/>
+      <c r="C7" s="5" t="inlineStr"/>
+      <c r="D7" s="5" t="inlineStr"/>
+      <c r="E7" s="5" t="inlineStr"/>
+      <c r="F7" s="5" t="inlineStr"/>
+      <c r="G7" s="5" t="inlineStr"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>